<commit_message>
using data driven testing in registration tests
</commit_message>
<xml_diff>
--- a/TC_BookStore/TestInputData/TestData.xlsx
+++ b/TC_BookStore/TestInputData/TestData.xlsx
@@ -7,39 +7,18 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="ResgiserUsers" sheetId="1" r:id="rId1"/>
+    <sheet name="ResgisterUsers" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t>Usdername</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>Re-Password</t>
-  </si>
-  <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
     <t>CCType</t>
   </si>
   <si>
@@ -59,6 +38,30 @@
   </si>
   <si>
     <t>Visa</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Repassword</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>phone</t>
   </si>
 </sst>
 </file>
@@ -132,12 +135,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -443,93 +445,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" s="1">
+        <v>123456</v>
+      </c>
+      <c r="D2" s="1">
+        <v>123456</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I2" s="1">
+        <v>190890383838</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>123456</v>
-      </c>
-      <c r="C2">
-        <v>123456</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="4">
-        <v>190890383838</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="4">
+      <c r="K2" s="1">
         <v>11233454555</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>